<commit_message>
Update colors, labels, title
</commit_message>
<xml_diff>
--- a/waterfall chart calculations_test.xlsx
+++ b/waterfall chart calculations_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cfan\Desktop\Plot\Matt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mshields\Documents\Projects\West Coast ports\Analysis\Supply chain\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{376176D3-0623-45FE-AFD2-B7C732E1D5F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{044463A7-4F98-415B-98BC-8DCEA0D40813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="10" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="baseline" sheetId="2" r:id="rId1"/>
@@ -402,7 +402,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -24520,20 +24520,20 @@
   <dimension ref="B2:H52"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
-    <col min="4" max="5" width="15.28515625" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.1796875" customWidth="1"/>
+    <col min="4" max="5" width="15.26953125" customWidth="1"/>
+    <col min="6" max="6" width="16.26953125" customWidth="1"/>
+    <col min="7" max="7" width="14.453125" customWidth="1"/>
+    <col min="8" max="8" width="10.26953125" style="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="15" thickBot="1">
+    <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="29" t="s">
         <v>0</v>
       </c>
@@ -24544,7 +24544,7 @@
       <c r="G2" s="29"/>
       <c r="H2" s="29"/>
     </row>
-    <row r="3" spans="2:8">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B3" s="23" t="s">
         <v>1</v>
       </c>
@@ -24567,7 +24567,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="2:8">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>8</v>
       </c>
@@ -24583,7 +24583,7 @@
       <c r="G4" s="7"/>
       <c r="H4" s="21"/>
     </row>
-    <row r="5" spans="2:8">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>9</v>
       </c>
@@ -24603,7 +24603,7 @@
       <c r="G5" s="7"/>
       <c r="H5" s="22"/>
     </row>
-    <row r="6" spans="2:8">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -24623,7 +24623,7 @@
       <c r="G6" s="7"/>
       <c r="H6" s="22"/>
     </row>
-    <row r="7" spans="2:8">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>11</v>
       </c>
@@ -24643,7 +24643,7 @@
       <c r="G7" s="7"/>
       <c r="H7" s="22"/>
     </row>
-    <row r="8" spans="2:8">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>12</v>
       </c>
@@ -24663,7 +24663,7 @@
       </c>
       <c r="H8" s="22"/>
     </row>
-    <row r="9" spans="2:8">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>13</v>
       </c>
@@ -24677,7 +24677,7 @@
       <c r="G9" s="7"/>
       <c r="H9" s="21"/>
     </row>
-    <row r="10" spans="2:8">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>14</v>
       </c>
@@ -24697,7 +24697,7 @@
       </c>
       <c r="H10" s="21"/>
     </row>
-    <row r="11" spans="2:8">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>15</v>
       </c>
@@ -24711,7 +24711,7 @@
       <c r="G11" s="8"/>
       <c r="H11" s="21"/>
     </row>
-    <row r="12" spans="2:8">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
@@ -24719,7 +24719,7 @@
       <c r="G12" s="8"/>
       <c r="H12" s="21"/>
     </row>
-    <row r="13" spans="2:8">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>16</v>
       </c>
@@ -24732,7 +24732,7 @@
       <c r="G13" s="8"/>
       <c r="H13" s="21"/>
     </row>
-    <row r="14" spans="2:8">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>17</v>
       </c>
@@ -24746,7 +24746,7 @@
       <c r="G14" s="8"/>
       <c r="H14" s="21"/>
     </row>
-    <row r="21" spans="2:8" ht="15" thickBot="1">
+    <row r="21" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B21" s="29" t="s">
         <v>18</v>
       </c>
@@ -24757,7 +24757,7 @@
       <c r="G21" s="29"/>
       <c r="H21" s="29"/>
     </row>
-    <row r="22" spans="2:8">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B22" s="23" t="s">
         <v>1</v>
       </c>
@@ -24780,7 +24780,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="2:8">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>8</v>
       </c>
@@ -24796,7 +24796,7 @@
       <c r="G23" s="7"/>
       <c r="H23" s="21"/>
     </row>
-    <row r="24" spans="2:8">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>9</v>
       </c>
@@ -24816,7 +24816,7 @@
       <c r="G24" s="7"/>
       <c r="H24" s="22"/>
     </row>
-    <row r="25" spans="2:8">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>10</v>
       </c>
@@ -24836,7 +24836,7 @@
       <c r="G25" s="7"/>
       <c r="H25" s="22"/>
     </row>
-    <row r="26" spans="2:8">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>11</v>
       </c>
@@ -24856,7 +24856,7 @@
       <c r="G26" s="7"/>
       <c r="H26" s="22"/>
     </row>
-    <row r="27" spans="2:8">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>19</v>
       </c>
@@ -24876,7 +24876,7 @@
       </c>
       <c r="H27" s="22"/>
     </row>
-    <row r="28" spans="2:8">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>20</v>
       </c>
@@ -24890,7 +24890,7 @@
       <c r="G28" s="7"/>
       <c r="H28" s="21"/>
     </row>
-    <row r="29" spans="2:8">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
         <v>14</v>
       </c>
@@ -24910,7 +24910,7 @@
       </c>
       <c r="H29" s="21"/>
     </row>
-    <row r="30" spans="2:8">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>21</v>
       </c>
@@ -24924,7 +24924,7 @@
       <c r="G30" s="8"/>
       <c r="H30" s="21"/>
     </row>
-    <row r="31" spans="2:8">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
@@ -24932,7 +24932,7 @@
       <c r="G31" s="8"/>
       <c r="H31" s="21"/>
     </row>
-    <row r="32" spans="2:8">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>16</v>
       </c>
@@ -24945,7 +24945,7 @@
       <c r="G32" s="8"/>
       <c r="H32" s="21"/>
     </row>
-    <row r="33" spans="2:8">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
         <v>17</v>
       </c>
@@ -24959,7 +24959,7 @@
       <c r="G33" s="8"/>
       <c r="H33" s="21"/>
     </row>
-    <row r="40" spans="2:8" ht="15" thickBot="1">
+    <row r="40" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B40" s="29" t="s">
         <v>22</v>
       </c>
@@ -24970,7 +24970,7 @@
       <c r="G40" s="29"/>
       <c r="H40" s="29"/>
     </row>
-    <row r="41" spans="2:8">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B41" s="23" t="s">
         <v>1</v>
       </c>
@@ -24993,7 +24993,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="2:8">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B42" t="s">
         <v>8</v>
       </c>
@@ -25009,7 +25009,7 @@
       <c r="G42" s="7"/>
       <c r="H42" s="21"/>
     </row>
-    <row r="43" spans="2:8">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B43" t="s">
         <v>9</v>
       </c>
@@ -25029,7 +25029,7 @@
       <c r="G43" s="7"/>
       <c r="H43" s="22"/>
     </row>
-    <row r="44" spans="2:8">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B44" t="s">
         <v>10</v>
       </c>
@@ -25049,7 +25049,7 @@
       <c r="G44" s="7"/>
       <c r="H44" s="22"/>
     </row>
-    <row r="45" spans="2:8">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B45" t="s">
         <v>11</v>
       </c>
@@ -25069,7 +25069,7 @@
       <c r="G45" s="7"/>
       <c r="H45" s="22"/>
     </row>
-    <row r="46" spans="2:8">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
         <v>19</v>
       </c>
@@ -25089,7 +25089,7 @@
       </c>
       <c r="H46" s="22"/>
     </row>
-    <row r="47" spans="2:8">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B47" t="s">
         <v>23</v>
       </c>
@@ -25103,7 +25103,7 @@
       <c r="G47" s="7"/>
       <c r="H47" s="21"/>
     </row>
-    <row r="48" spans="2:8">
+    <row r="48" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B48" t="s">
         <v>14</v>
       </c>
@@ -25123,7 +25123,7 @@
       </c>
       <c r="H48" s="21"/>
     </row>
-    <row r="49" spans="2:8">
+    <row r="49" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B49" t="s">
         <v>24</v>
       </c>
@@ -25137,7 +25137,7 @@
       <c r="G49" s="8"/>
       <c r="H49" s="21"/>
     </row>
-    <row r="50" spans="2:8">
+    <row r="50" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C50" s="8"/>
       <c r="D50" s="8"/>
       <c r="E50" s="8"/>
@@ -25145,7 +25145,7 @@
       <c r="G50" s="8"/>
       <c r="H50" s="21"/>
     </row>
-    <row r="51" spans="2:8">
+    <row r="51" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B51" t="s">
         <v>16</v>
       </c>
@@ -25158,7 +25158,7 @@
       <c r="G51" s="8"/>
       <c r="H51" s="21"/>
     </row>
-    <row r="52" spans="2:8">
+    <row r="52" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B52" t="s">
         <v>17</v>
       </c>
@@ -25187,17 +25187,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AD60C66-AC5C-4361-9AF3-08627913F5D4}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="36.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>94</v>
       </c>
@@ -25205,7 +25205,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>96</v>
       </c>
@@ -25213,7 +25213,7 @@
         <v>2216.36</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>97</v>
       </c>
@@ -25221,7 +25221,7 @@
         <v>378.18</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>98</v>
       </c>
@@ -25229,7 +25229,7 @@
         <v>223.18</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>99</v>
       </c>
@@ -25237,7 +25237,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>100</v>
       </c>
@@ -25245,7 +25245,7 @@
         <v>-661</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="27" t="s">
         <v>101</v>
       </c>
@@ -25254,7 +25254,7 @@
         <v>2262.7199999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>102</v>
       </c>
@@ -25263,7 +25263,7 @@
         <v>-226.27199999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>103</v>
       </c>
@@ -25281,17 +25281,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3225781-4E14-495E-8072-139066F77D75}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="35.28515625" customWidth="1"/>
-    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.26953125" customWidth="1"/>
+    <col min="2" max="2" width="7.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>94</v>
       </c>
@@ -25299,7 +25299,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>96</v>
       </c>
@@ -25307,7 +25307,7 @@
         <v>2216.36</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>97</v>
       </c>
@@ -25315,7 +25315,7 @@
         <v>378.18</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>98</v>
       </c>
@@ -25323,7 +25323,7 @@
         <v>223.18</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>99</v>
       </c>
@@ -25331,7 +25331,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="28" t="s">
         <v>104</v>
       </c>
@@ -25339,7 +25339,7 @@
         <v>-661</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>101</v>
       </c>
@@ -25348,7 +25348,7 @@
         <v>2262.7199999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="28" t="s">
         <v>100</v>
       </c>
@@ -25356,7 +25356,7 @@
         <v>202.89</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>103</v>
       </c>
@@ -25380,13 +25380,13 @@
       <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>94</v>
       </c>
@@ -25394,7 +25394,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -25402,7 +25402,7 @@
         <v>2202</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>105</v>
       </c>
@@ -25411,7 +25411,7 @@
         <v>2580</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>88</v>
       </c>
@@ -25420,7 +25420,7 @@
         <v>2817</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>89</v>
       </c>
@@ -25429,7 +25429,7 @@
         <v>2923</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>106</v>
       </c>
@@ -25438,7 +25438,7 @@
         <v>2262</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -25447,7 +25447,7 @@
         <v>2262</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>107</v>
       </c>
@@ -25456,7 +25456,7 @@
         <v>2036</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -25478,17 +25478,17 @@
       <selection activeCell="C4" sqref="C4:D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
-    <col min="4" max="5" width="15.28515625" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.1796875" customWidth="1"/>
+    <col min="4" max="5" width="15.26953125" customWidth="1"/>
+    <col min="6" max="6" width="16.26953125" customWidth="1"/>
+    <col min="7" max="7" width="14.453125" customWidth="1"/>
+    <col min="8" max="8" width="10.26953125" style="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="15" thickBot="1">
+    <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="29" t="s">
         <v>0</v>
       </c>
@@ -25499,7 +25499,7 @@
       <c r="G2" s="29"/>
       <c r="H2" s="29"/>
     </row>
-    <row r="3" spans="2:8">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B3" s="23" t="s">
         <v>1</v>
       </c>
@@ -25522,7 +25522,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="2:8">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>25</v>
       </c>
@@ -25538,7 +25538,7 @@
       <c r="G4" s="7"/>
       <c r="H4" s="21"/>
     </row>
-    <row r="5" spans="2:8">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>9</v>
       </c>
@@ -25558,7 +25558,7 @@
       <c r="G5" s="7"/>
       <c r="H5" s="22"/>
     </row>
-    <row r="6" spans="2:8">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -25578,7 +25578,7 @@
       <c r="G6" s="7"/>
       <c r="H6" s="22"/>
     </row>
-    <row r="7" spans="2:8">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>11</v>
       </c>
@@ -25598,7 +25598,7 @@
       <c r="G7" s="7"/>
       <c r="H7" s="22"/>
     </row>
-    <row r="8" spans="2:8">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>12</v>
       </c>
@@ -25618,7 +25618,7 @@
       </c>
       <c r="H8" s="22"/>
     </row>
-    <row r="9" spans="2:8">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>13</v>
       </c>
@@ -25632,7 +25632,7 @@
       <c r="G9" s="7"/>
       <c r="H9" s="21"/>
     </row>
-    <row r="10" spans="2:8">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>14</v>
       </c>
@@ -25652,7 +25652,7 @@
       </c>
       <c r="H10" s="21"/>
     </row>
-    <row r="11" spans="2:8">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>15</v>
       </c>
@@ -25666,7 +25666,7 @@
       <c r="G11" s="8"/>
       <c r="H11" s="21"/>
     </row>
-    <row r="12" spans="2:8">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
@@ -25674,7 +25674,7 @@
       <c r="G12" s="8"/>
       <c r="H12" s="21"/>
     </row>
-    <row r="13" spans="2:8">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>16</v>
       </c>
@@ -25687,7 +25687,7 @@
       <c r="G13" s="8"/>
       <c r="H13" s="21"/>
     </row>
-    <row r="14" spans="2:8">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>17</v>
       </c>
@@ -25701,7 +25701,7 @@
       <c r="G14" s="8"/>
       <c r="H14" s="21"/>
     </row>
-    <row r="21" spans="2:8" ht="15" thickBot="1">
+    <row r="21" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B21" s="29" t="s">
         <v>18</v>
       </c>
@@ -25712,7 +25712,7 @@
       <c r="G21" s="29"/>
       <c r="H21" s="29"/>
     </row>
-    <row r="22" spans="2:8">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B22" s="23" t="s">
         <v>1</v>
       </c>
@@ -25735,7 +25735,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="2:8">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>8</v>
       </c>
@@ -25751,7 +25751,7 @@
       <c r="G23" s="7"/>
       <c r="H23" s="21"/>
     </row>
-    <row r="24" spans="2:8">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>9</v>
       </c>
@@ -25771,7 +25771,7 @@
       <c r="G24" s="7"/>
       <c r="H24" s="22"/>
     </row>
-    <row r="25" spans="2:8">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>10</v>
       </c>
@@ -25791,7 +25791,7 @@
       <c r="G25" s="7"/>
       <c r="H25" s="22"/>
     </row>
-    <row r="26" spans="2:8">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>11</v>
       </c>
@@ -25811,7 +25811,7 @@
       <c r="G26" s="7"/>
       <c r="H26" s="22"/>
     </row>
-    <row r="27" spans="2:8">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>19</v>
       </c>
@@ -25831,7 +25831,7 @@
       </c>
       <c r="H27" s="22"/>
     </row>
-    <row r="28" spans="2:8">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>20</v>
       </c>
@@ -25845,7 +25845,7 @@
       <c r="G28" s="7"/>
       <c r="H28" s="21"/>
     </row>
-    <row r="29" spans="2:8">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
         <v>14</v>
       </c>
@@ -25865,7 +25865,7 @@
       </c>
       <c r="H29" s="21"/>
     </row>
-    <row r="30" spans="2:8">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>21</v>
       </c>
@@ -25879,7 +25879,7 @@
       <c r="G30" s="8"/>
       <c r="H30" s="21"/>
     </row>
-    <row r="31" spans="2:8">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
@@ -25887,7 +25887,7 @@
       <c r="G31" s="8"/>
       <c r="H31" s="21"/>
     </row>
-    <row r="32" spans="2:8">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>16</v>
       </c>
@@ -25900,7 +25900,7 @@
       <c r="G32" s="8"/>
       <c r="H32" s="21"/>
     </row>
-    <row r="33" spans="2:8">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
         <v>17</v>
       </c>
@@ -25914,7 +25914,7 @@
       <c r="G33" s="8"/>
       <c r="H33" s="21"/>
     </row>
-    <row r="40" spans="2:8" ht="15" thickBot="1">
+    <row r="40" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B40" s="29" t="s">
         <v>22</v>
       </c>
@@ -25925,7 +25925,7 @@
       <c r="G40" s="29"/>
       <c r="H40" s="29"/>
     </row>
-    <row r="41" spans="2:8">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B41" s="23" t="s">
         <v>1</v>
       </c>
@@ -25948,7 +25948,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="2:8">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B42" t="s">
         <v>8</v>
       </c>
@@ -25964,7 +25964,7 @@
       <c r="G42" s="7"/>
       <c r="H42" s="21"/>
     </row>
-    <row r="43" spans="2:8">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B43" t="s">
         <v>9</v>
       </c>
@@ -25984,7 +25984,7 @@
       <c r="G43" s="7"/>
       <c r="H43" s="22"/>
     </row>
-    <row r="44" spans="2:8">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B44" t="s">
         <v>10</v>
       </c>
@@ -26004,7 +26004,7 @@
       <c r="G44" s="7"/>
       <c r="H44" s="22"/>
     </row>
-    <row r="45" spans="2:8">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B45" t="s">
         <v>11</v>
       </c>
@@ -26024,7 +26024,7 @@
       <c r="G45" s="7"/>
       <c r="H45" s="22"/>
     </row>
-    <row r="46" spans="2:8">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
         <v>19</v>
       </c>
@@ -26044,7 +26044,7 @@
       </c>
       <c r="H46" s="22"/>
     </row>
-    <row r="47" spans="2:8">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B47" t="s">
         <v>23</v>
       </c>
@@ -26058,7 +26058,7 @@
       <c r="G47" s="7"/>
       <c r="H47" s="21"/>
     </row>
-    <row r="48" spans="2:8">
+    <row r="48" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B48" t="s">
         <v>14</v>
       </c>
@@ -26078,7 +26078,7 @@
       </c>
       <c r="H48" s="21"/>
     </row>
-    <row r="49" spans="2:8">
+    <row r="49" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B49" t="s">
         <v>24</v>
       </c>
@@ -26092,7 +26092,7 @@
       <c r="G49" s="8"/>
       <c r="H49" s="21"/>
     </row>
-    <row r="50" spans="2:8">
+    <row r="50" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C50" s="8"/>
       <c r="D50" s="8"/>
       <c r="E50" s="8"/>
@@ -26100,7 +26100,7 @@
       <c r="G50" s="8"/>
       <c r="H50" s="21"/>
     </row>
-    <row r="51" spans="2:8">
+    <row r="51" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B51" t="s">
         <v>16</v>
       </c>
@@ -26113,7 +26113,7 @@
       <c r="G51" s="8"/>
       <c r="H51" s="21"/>
     </row>
-    <row r="52" spans="2:8">
+    <row r="52" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B52" t="s">
         <v>17</v>
       </c>
@@ -26146,17 +26146,17 @@
       <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1796875" customWidth="1"/>
+    <col min="5" max="5" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>26</v>
       </c>
@@ -26167,7 +26167,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="2:7">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>29</v>
       </c>
@@ -26186,7 +26186,7 @@
         <v>748.79100000000005</v>
       </c>
     </row>
-    <row r="4" spans="2:7">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>30</v>
       </c>
@@ -26205,7 +26205,7 @@
         <v>1189.7820000000002</v>
       </c>
     </row>
-    <row r="5" spans="2:7">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>31</v>
       </c>
@@ -26224,7 +26224,7 @@
         <v>93.933000000000007</v>
       </c>
     </row>
-    <row r="6" spans="2:7">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>32</v>
       </c>
@@ -26257,16 +26257,16 @@
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
-    <col min="4" max="5" width="15.28515625" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="32.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.1796875" customWidth="1"/>
+    <col min="4" max="5" width="15.26953125" customWidth="1"/>
+    <col min="6" max="6" width="16.26953125" customWidth="1"/>
+    <col min="7" max="7" width="14.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -26286,7 +26286,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:15">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>33</v>
       </c>
@@ -26302,7 +26302,7 @@
       <c r="G3" s="7"/>
       <c r="H3" s="8"/>
     </row>
-    <row r="4" spans="2:15">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>9</v>
       </c>
@@ -26322,7 +26322,7 @@
       <c r="G4" s="7"/>
       <c r="H4" s="9"/>
     </row>
-    <row r="5" spans="2:15">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>10</v>
       </c>
@@ -26342,7 +26342,7 @@
       <c r="G5" s="7"/>
       <c r="H5" s="9"/>
     </row>
-    <row r="6" spans="2:15">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>11</v>
       </c>
@@ -26362,7 +26362,7 @@
       <c r="G6" s="7"/>
       <c r="H6" s="9"/>
     </row>
-    <row r="7" spans="2:15">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>34</v>
       </c>
@@ -26382,7 +26382,7 @@
       </c>
       <c r="H7" s="9"/>
     </row>
-    <row r="8" spans="2:15">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>35</v>
       </c>
@@ -26396,7 +26396,7 @@
       <c r="G8" s="7"/>
       <c r="H8" s="8"/>
     </row>
-    <row r="9" spans="2:15">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>17</v>
       </c>
@@ -26416,7 +26416,7 @@
       </c>
       <c r="H9" s="8"/>
     </row>
-    <row r="10" spans="2:15">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>36</v>
       </c>
@@ -26430,7 +26430,7 @@
       <c r="G10" s="7"/>
       <c r="H10" s="8"/>
     </row>
-    <row r="11" spans="2:15">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>37</v>
       </c>
@@ -26441,7 +26441,7 @@
       <c r="G11" s="7"/>
       <c r="H11" s="8"/>
     </row>
-    <row r="12" spans="2:15">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>38</v>
       </c>
@@ -26456,7 +26456,7 @@
       <c r="N12" s="31"/>
       <c r="O12" s="31"/>
     </row>
-    <row r="13" spans="2:15">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
@@ -26470,7 +26470,7 @@
       <c r="N13" s="31"/>
       <c r="O13" s="31"/>
     </row>
-    <row r="14" spans="2:15">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>16</v>
       </c>
@@ -26489,7 +26489,7 @@
       <c r="N14" s="31"/>
       <c r="O14" s="31"/>
     </row>
-    <row r="15" spans="2:15">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>17</v>
       </c>
@@ -26509,7 +26509,7 @@
       <c r="N15" s="31"/>
       <c r="O15" s="31"/>
     </row>
-    <row r="16" spans="2:15">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.35">
       <c r="J16" s="31"/>
       <c r="K16" s="31"/>
       <c r="L16" s="31"/>
@@ -26517,7 +26517,7 @@
       <c r="N16" s="31"/>
       <c r="O16" s="31"/>
     </row>
-    <row r="17" spans="2:3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>40</v>
       </c>
@@ -26525,7 +26525,7 @@
         <v>2074</v>
       </c>
     </row>
-    <row r="18" spans="2:3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>41</v>
       </c>
@@ -26551,17 +26551,17 @@
       <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
-    <col min="4" max="5" width="15.28515625" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" style="20" customWidth="1"/>
+    <col min="2" max="2" width="27.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.1796875" customWidth="1"/>
+    <col min="4" max="5" width="15.26953125" customWidth="1"/>
+    <col min="6" max="6" width="16.26953125" customWidth="1"/>
+    <col min="7" max="7" width="14.453125" customWidth="1"/>
+    <col min="8" max="8" width="13.1796875" style="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="15" thickBot="1">
+    <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="29" t="s">
         <v>18</v>
       </c>
@@ -26572,7 +26572,7 @@
       <c r="G2" s="29"/>
       <c r="H2" s="29"/>
     </row>
-    <row r="3" spans="2:8">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B3" s="23" t="s">
         <v>1</v>
       </c>
@@ -26595,7 +26595,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="2:8">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>8</v>
       </c>
@@ -26610,7 +26610,7 @@
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
     </row>
-    <row r="5" spans="2:8">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>9</v>
       </c>
@@ -26630,7 +26630,7 @@
       <c r="G5" s="7"/>
       <c r="H5" s="25"/>
     </row>
-    <row r="6" spans="2:8">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -26653,7 +26653,7 @@
         <v>202.88999999999987</v>
       </c>
     </row>
-    <row r="7" spans="2:8">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>11</v>
       </c>
@@ -26676,7 +26676,7 @@
         <v>4.7599999999999909</v>
       </c>
     </row>
-    <row r="8" spans="2:8">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>19</v>
       </c>
@@ -26696,7 +26696,7 @@
       </c>
       <c r="H8" s="25"/>
     </row>
-    <row r="9" spans="2:8">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>21</v>
       </c>
@@ -26709,7 +26709,7 @@
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
     </row>
-    <row r="10" spans="2:8">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>42</v>
       </c>
@@ -26728,7 +26728,7 @@
       </c>
       <c r="G10" s="7"/>
     </row>
-    <row r="11" spans="2:8">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>43</v>
       </c>
@@ -26741,28 +26741,28 @@
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
     </row>
-    <row r="12" spans="2:8">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
     </row>
-    <row r="13" spans="2:8">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C13" s="7"/>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
     </row>
-    <row r="14" spans="2:8">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
     </row>
-    <row r="21" spans="2:8" ht="15" thickBot="1">
+    <row r="21" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B21" s="29" t="s">
         <v>22</v>
       </c>
@@ -26773,7 +26773,7 @@
       <c r="G21" s="29"/>
       <c r="H21" s="29"/>
     </row>
-    <row r="22" spans="2:8">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B22" s="23" t="s">
         <v>1</v>
       </c>
@@ -26796,7 +26796,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="2:8">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>8</v>
       </c>
@@ -26811,7 +26811,7 @@
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
     </row>
-    <row r="24" spans="2:8">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>9</v>
       </c>
@@ -26831,7 +26831,7 @@
       <c r="G24" s="7"/>
       <c r="H24" s="25"/>
     </row>
-    <row r="25" spans="2:8">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>10</v>
       </c>
@@ -26854,7 +26854,7 @@
         <v>202.88999999999987</v>
       </c>
     </row>
-    <row r="26" spans="2:8">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>11</v>
       </c>
@@ -26877,7 +26877,7 @@
         <v>4.7600000000000051</v>
       </c>
     </row>
-    <row r="27" spans="2:8">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>19</v>
       </c>
@@ -26897,7 +26897,7 @@
       </c>
       <c r="H27" s="25"/>
     </row>
-    <row r="28" spans="2:8">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>44</v>
       </c>
@@ -26910,7 +26910,7 @@
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
     </row>
-    <row r="29" spans="2:8">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
         <v>42</v>
       </c>
@@ -26928,7 +26928,7 @@
         <v>207.64999999999986</v>
       </c>
     </row>
-    <row r="30" spans="2:8">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>45</v>
       </c>
@@ -26941,7 +26941,7 @@
       <c r="F30" s="8"/>
       <c r="G30" s="8"/>
     </row>
-    <row r="31" spans="2:8">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
@@ -26966,17 +26966,17 @@
       <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
-    <col min="4" max="5" width="15.28515625" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" style="20" customWidth="1"/>
+    <col min="2" max="2" width="27.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.1796875" customWidth="1"/>
+    <col min="4" max="5" width="15.26953125" customWidth="1"/>
+    <col min="6" max="6" width="16.26953125" customWidth="1"/>
+    <col min="7" max="7" width="14.453125" customWidth="1"/>
+    <col min="8" max="8" width="13.1796875" style="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="15" thickBot="1">
+    <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B1" s="29" t="s">
         <v>0</v>
       </c>
@@ -26987,7 +26987,7 @@
       <c r="G1" s="29"/>
       <c r="H1" s="29"/>
     </row>
-    <row r="2" spans="2:8">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B2" s="23" t="s">
         <v>1</v>
       </c>
@@ -27010,7 +27010,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="2:8">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>25</v>
       </c>
@@ -27025,7 +27025,7 @@
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
     </row>
-    <row r="4" spans="2:8">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>9</v>
       </c>
@@ -27045,7 +27045,7 @@
       <c r="G4" s="7"/>
       <c r="H4" s="25"/>
     </row>
-    <row r="5" spans="2:8">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>10</v>
       </c>
@@ -27068,7 +27068,7 @@
         <v>202.88999999999987</v>
       </c>
     </row>
-    <row r="6" spans="2:8">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>11</v>
       </c>
@@ -27091,7 +27091,7 @@
         <v>4.7599999999999909</v>
       </c>
     </row>
-    <row r="7" spans="2:8">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>19</v>
       </c>
@@ -27111,7 +27111,7 @@
       </c>
       <c r="H7" s="25"/>
     </row>
-    <row r="8" spans="2:8">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>15</v>
       </c>
@@ -27124,7 +27124,7 @@
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
     </row>
-    <row r="9" spans="2:8">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>42</v>
       </c>
@@ -27143,7 +27143,7 @@
       </c>
       <c r="G9" s="7"/>
     </row>
-    <row r="10" spans="2:8">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>46</v>
       </c>
@@ -27156,28 +27156,28 @@
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
     </row>
-    <row r="11" spans="2:8">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
     </row>
-    <row r="12" spans="2:8">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C12" s="7"/>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
     </row>
-    <row r="13" spans="2:8">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
     </row>
-    <row r="19" spans="2:8" ht="15" thickBot="1">
+    <row r="19" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B19" s="29" t="s">
         <v>18</v>
       </c>
@@ -27188,7 +27188,7 @@
       <c r="G19" s="29"/>
       <c r="H19" s="29"/>
     </row>
-    <row r="20" spans="2:8">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B20" s="23" t="s">
         <v>1</v>
       </c>
@@ -27211,7 +27211,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="2:8">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>8</v>
       </c>
@@ -27226,7 +27226,7 @@
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
     </row>
-    <row r="22" spans="2:8">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>9</v>
       </c>
@@ -27246,7 +27246,7 @@
       <c r="G22" s="7"/>
       <c r="H22" s="25"/>
     </row>
-    <row r="23" spans="2:8">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>10</v>
       </c>
@@ -27269,7 +27269,7 @@
         <v>202.88999999999987</v>
       </c>
     </row>
-    <row r="24" spans="2:8">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>11</v>
       </c>
@@ -27292,7 +27292,7 @@
         <v>4.7599999999999909</v>
       </c>
     </row>
-    <row r="25" spans="2:8">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>19</v>
       </c>
@@ -27312,7 +27312,7 @@
       </c>
       <c r="H25" s="25"/>
     </row>
-    <row r="26" spans="2:8">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>21</v>
       </c>
@@ -27325,7 +27325,7 @@
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
     </row>
-    <row r="27" spans="2:8">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>42</v>
       </c>
@@ -27344,7 +27344,7 @@
       </c>
       <c r="G27" s="7"/>
     </row>
-    <row r="28" spans="2:8">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>43</v>
       </c>
@@ -27357,28 +27357,28 @@
       <c r="F28" s="8"/>
       <c r="G28" s="8"/>
     </row>
-    <row r="29" spans="2:8">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
       <c r="E29" s="8"/>
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
     </row>
-    <row r="30" spans="2:8">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C30" s="7"/>
       <c r="D30" s="8"/>
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
       <c r="G30" s="8"/>
     </row>
-    <row r="31" spans="2:8">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
       <c r="G31" s="8"/>
     </row>
-    <row r="38" spans="2:8" ht="15" thickBot="1">
+    <row r="38" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B38" s="29" t="s">
         <v>22</v>
       </c>
@@ -27389,7 +27389,7 @@
       <c r="G38" s="29"/>
       <c r="H38" s="29"/>
     </row>
-    <row r="39" spans="2:8">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B39" s="23" t="s">
         <v>1</v>
       </c>
@@ -27412,7 +27412,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="2:8">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B40" t="s">
         <v>8</v>
       </c>
@@ -27427,7 +27427,7 @@
       <c r="F40" s="7"/>
       <c r="G40" s="7"/>
     </row>
-    <row r="41" spans="2:8">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
         <v>9</v>
       </c>
@@ -27447,7 +27447,7 @@
       <c r="G41" s="7"/>
       <c r="H41" s="25"/>
     </row>
-    <row r="42" spans="2:8">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B42" t="s">
         <v>10</v>
       </c>
@@ -27470,7 +27470,7 @@
         <v>202.88999999999987</v>
       </c>
     </row>
-    <row r="43" spans="2:8">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B43" t="s">
         <v>11</v>
       </c>
@@ -27493,7 +27493,7 @@
         <v>4.7600000000000051</v>
       </c>
     </row>
-    <row r="44" spans="2:8">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B44" t="s">
         <v>19</v>
       </c>
@@ -27513,7 +27513,7 @@
       </c>
       <c r="H44" s="25"/>
     </row>
-    <row r="45" spans="2:8">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B45" t="s">
         <v>44</v>
       </c>
@@ -27526,7 +27526,7 @@
       <c r="F45" s="7"/>
       <c r="G45" s="7"/>
     </row>
-    <row r="46" spans="2:8">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
         <v>42</v>
       </c>
@@ -27544,7 +27544,7 @@
         <v>207.64999999999986</v>
       </c>
     </row>
-    <row r="47" spans="2:8">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B47" t="s">
         <v>45</v>
       </c>
@@ -27557,7 +27557,7 @@
       <c r="F47" s="8"/>
       <c r="G47" s="8"/>
     </row>
-    <row r="48" spans="2:8">
+    <row r="48" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C48" s="8"/>
       <c r="D48" s="8"/>
       <c r="E48" s="8"/>
@@ -27583,19 +27583,19 @@
       <selection activeCell="M1" sqref="M1:M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="32.26953125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:20">
+    <row r="3" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B3" s="10" t="s">
         <v>33</v>
       </c>
@@ -27618,7 +27618,7 @@
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
     </row>
-    <row r="4" spans="2:20">
+    <row r="4" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B4" s="11" t="s">
         <v>47</v>
       </c>
@@ -27677,7 +27677,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="2:20">
+    <row r="5" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
         <v>63</v>
       </c>
@@ -27730,7 +27730,7 @@
         <v>112133.83</v>
       </c>
     </row>
-    <row r="6" spans="2:20">
+    <row r="6" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
         <v>65</v>
       </c>
@@ -27783,7 +27783,7 @@
         <v>79153.289999999994</v>
       </c>
     </row>
-    <row r="7" spans="2:20">
+    <row r="7" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B7" s="2" t="s">
         <v>66</v>
       </c>
@@ -27836,7 +27836,7 @@
         <v>92345.5</v>
       </c>
     </row>
-    <row r="8" spans="2:20">
+    <row r="8" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B8" s="2" t="s">
         <v>67</v>
       </c>
@@ -27889,7 +27889,7 @@
         <v>224267.65</v>
       </c>
     </row>
-    <row r="9" spans="2:20">
+    <row r="9" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">
         <v>68</v>
       </c>
@@ -27938,7 +27938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:20">
+    <row r="10" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B10" s="2" t="s">
         <v>70</v>
       </c>
@@ -27991,7 +27991,7 @@
         <v>6596.11</v>
       </c>
     </row>
-    <row r="11" spans="2:20">
+    <row r="11" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B11" s="2" t="s">
         <v>71</v>
       </c>
@@ -28044,7 +28044,7 @@
         <v>32980.54</v>
       </c>
     </row>
-    <row r="12" spans="2:20">
+    <row r="12" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B12" s="2" t="s">
         <v>72</v>
       </c>
@@ -28097,7 +28097,7 @@
         <v>92345.5</v>
       </c>
     </row>
-    <row r="13" spans="2:20">
+    <row r="13" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B13" s="2" t="s">
         <v>73</v>
       </c>
@@ -28150,7 +28150,7 @@
         <v>13192.21</v>
       </c>
     </row>
-    <row r="14" spans="2:20">
+    <row r="14" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B14" s="2" t="s">
         <v>74</v>
       </c>
@@ -28203,7 +28203,7 @@
         <v>13192.21</v>
       </c>
     </row>
-    <row r="15" spans="2:20">
+    <row r="15" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B15" s="2" t="s">
         <v>75</v>
       </c>
@@ -28256,7 +28256,7 @@
         <v>6596.11</v>
       </c>
     </row>
-    <row r="16" spans="2:20">
+    <row r="16" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B16" s="2" t="s">
         <v>76</v>
       </c>
@@ -28297,7 +28297,7 @@
         <v>672802.96</v>
       </c>
     </row>
-    <row r="18" spans="2:20">
+    <row r="18" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B18" s="10" t="s">
         <v>77</v>
       </c>
@@ -28320,7 +28320,7 @@
       <c r="S18" s="1"/>
       <c r="T18" s="1"/>
     </row>
-    <row r="19" spans="2:20">
+    <row r="19" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B19" s="11" t="s">
         <v>47</v>
       </c>
@@ -28379,7 +28379,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="2:20">
+    <row r="20" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B20" s="2" t="s">
         <v>63</v>
       </c>
@@ -28438,7 +28438,7 @@
         <v>5096.99</v>
       </c>
     </row>
-    <row r="21" spans="2:20">
+    <row r="21" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B21" s="2" t="s">
         <v>65</v>
       </c>
@@ -28497,7 +28497,7 @@
         <v>3597.88</v>
       </c>
     </row>
-    <row r="22" spans="2:20">
+    <row r="22" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B22" s="2" t="s">
         <v>66</v>
       </c>
@@ -28556,7 +28556,7 @@
         <v>4197.5200000000004</v>
       </c>
     </row>
-    <row r="23" spans="2:20">
+    <row r="23" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B23" s="2" t="s">
         <v>67</v>
       </c>
@@ -28611,7 +28611,7 @@
         <v>10193.98</v>
       </c>
     </row>
-    <row r="24" spans="2:20">
+    <row r="24" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B24" s="2" t="s">
         <v>68</v>
       </c>
@@ -28666,7 +28666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:20">
+    <row r="25" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B25" s="2" t="s">
         <v>70</v>
       </c>
@@ -28725,7 +28725,7 @@
         <v>299.82</v>
       </c>
     </row>
-    <row r="26" spans="2:20">
+    <row r="26" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B26" s="2" t="s">
         <v>71</v>
       </c>
@@ -28784,7 +28784,7 @@
         <v>1499.12</v>
       </c>
     </row>
-    <row r="27" spans="2:20">
+    <row r="27" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B27" s="2" t="s">
         <v>72</v>
       </c>
@@ -28843,7 +28843,7 @@
         <v>4197.5200000000004</v>
       </c>
     </row>
-    <row r="28" spans="2:20">
+    <row r="28" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B28" s="2" t="s">
         <v>73</v>
       </c>
@@ -28902,7 +28902,7 @@
         <v>599.65</v>
       </c>
     </row>
-    <row r="29" spans="2:20">
+    <row r="29" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B29" s="2" t="s">
         <v>74</v>
       </c>
@@ -28961,7 +28961,7 @@
         <v>599.65</v>
       </c>
     </row>
-    <row r="30" spans="2:20">
+    <row r="30" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B30" s="2" t="s">
         <v>75</v>
       </c>
@@ -29020,7 +29020,7 @@
         <v>299.82</v>
       </c>
     </row>
-    <row r="31" spans="2:20">
+    <row r="31" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B31" s="2" t="s">
         <v>76</v>
       </c>
@@ -29063,7 +29063,7 @@
         <v>30581.95</v>
       </c>
     </row>
-    <row r="32" spans="2:20">
+    <row r="32" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -29088,7 +29088,7 @@
         <v>35475.07</v>
       </c>
     </row>
-    <row r="33" spans="2:20">
+    <row r="33" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B33" s="10" t="s">
         <v>77</v>
       </c>
@@ -29111,7 +29111,7 @@
       <c r="S33" s="1"/>
       <c r="T33" s="1"/>
     </row>
-    <row r="34" spans="2:20">
+    <row r="34" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B34" s="11" t="s">
         <v>47</v>
       </c>
@@ -29170,7 +29170,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="2:20">
+    <row r="35" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B35" s="2" t="s">
         <v>63</v>
       </c>
@@ -29229,7 +29229,7 @@
         <v>5096.99</v>
       </c>
     </row>
-    <row r="36" spans="2:20">
+    <row r="36" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B36" s="2" t="s">
         <v>65</v>
       </c>
@@ -29288,7 +29288,7 @@
         <v>3597.88</v>
       </c>
     </row>
-    <row r="37" spans="2:20">
+    <row r="37" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B37" s="2" t="s">
         <v>66</v>
       </c>
@@ -29347,7 +29347,7 @@
         <v>4197.5200000000004</v>
       </c>
     </row>
-    <row r="38" spans="2:20">
+    <row r="38" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B38" s="2" t="s">
         <v>67</v>
       </c>
@@ -29402,7 +29402,7 @@
         <v>10193.98</v>
       </c>
     </row>
-    <row r="39" spans="2:20">
+    <row r="39" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B39" s="2" t="s">
         <v>68</v>
       </c>
@@ -29457,7 +29457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:20">
+    <row r="40" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B40" s="2" t="s">
         <v>70</v>
       </c>
@@ -29516,7 +29516,7 @@
         <v>299.82</v>
       </c>
     </row>
-    <row r="41" spans="2:20">
+    <row r="41" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B41" s="2" t="s">
         <v>71</v>
       </c>
@@ -29575,7 +29575,7 @@
         <v>1499.12</v>
       </c>
     </row>
-    <row r="42" spans="2:20">
+    <row r="42" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B42" s="2" t="s">
         <v>72</v>
       </c>
@@ -29634,7 +29634,7 @@
         <v>4197.5200000000004</v>
       </c>
     </row>
-    <row r="43" spans="2:20">
+    <row r="43" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B43" s="2" t="s">
         <v>73</v>
       </c>
@@ -29693,7 +29693,7 @@
         <v>599.65</v>
       </c>
     </row>
-    <row r="44" spans="2:20">
+    <row r="44" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B44" s="2" t="s">
         <v>74</v>
       </c>
@@ -29752,7 +29752,7 @@
         <v>599.65</v>
       </c>
     </row>
-    <row r="45" spans="2:20">
+    <row r="45" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B45" s="2" t="s">
         <v>75</v>
       </c>
@@ -29811,7 +29811,7 @@
         <v>299.82</v>
       </c>
     </row>
-    <row r="46" spans="2:20">
+    <row r="46" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B46" s="2" t="s">
         <v>76</v>
       </c>
@@ -29854,7 +29854,7 @@
         <v>30581.95</v>
       </c>
     </row>
-    <row r="47" spans="2:20">
+    <row r="47" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
@@ -29879,14 +29879,14 @@
         <v>35475.07</v>
       </c>
     </row>
-    <row r="48" spans="2:20">
+    <row r="48" spans="2:20" x14ac:dyDescent="0.35">
       <c r="F48" s="13"/>
       <c r="G48" s="13"/>
       <c r="H48" s="13"/>
       <c r="O48" s="13"/>
       <c r="R48" s="13"/>
     </row>
-    <row r="49" spans="2:18">
+    <row r="49" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B49" s="1" t="s">
         <v>33</v>
       </c>
@@ -29909,7 +29909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:18">
+    <row r="50" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B50" s="1" t="s">
         <v>77</v>
       </c>
@@ -29934,7 +29934,7 @@
         <v>110.86</v>
       </c>
     </row>
-    <row r="51" spans="2:18">
+    <row r="51" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B51" s="1" t="s">
         <v>78</v>
       </c>
@@ -29959,7 +29959,7 @@
         <v>115.97</v>
       </c>
     </row>
-    <row r="53" spans="2:18">
+    <row r="53" spans="2:18" x14ac:dyDescent="0.35">
       <c r="F53" s="13">
         <f>F50-F49</f>
         <v>453.81</v>
@@ -29981,7 +29981,7 @@
         <v>110.86</v>
       </c>
     </row>
-    <row r="54" spans="2:18">
+    <row r="54" spans="2:18" x14ac:dyDescent="0.35">
       <c r="F54" s="13">
         <f>F51-F50</f>
         <v>0</v>
@@ -30016,18 +30016,18 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.81640625" customWidth="1"/>
     <col min="3" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7265625" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>79</v>
       </c>
@@ -30056,7 +30056,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -30071,7 +30071,7 @@
       <c r="H2" s="6"/>
       <c r="I2" s="4"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -30090,7 +30090,7 @@
       <c r="H3" s="6"/>
       <c r="I3" s="4"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>88</v>
       </c>
@@ -30109,7 +30109,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="4"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>89</v>
       </c>
@@ -30130,7 +30130,7 @@
       <c r="H5" s="6"/>
       <c r="I5" s="4"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>84</v>
       </c>
@@ -30149,7 +30149,7 @@
       </c>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>90</v>
       </c>
@@ -30167,7 +30167,7 @@
       </c>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>91</v>
       </c>
@@ -30183,7 +30183,7 @@
       <c r="H8" s="6"/>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -30191,7 +30191,7 @@
         <v>2311</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -30200,55 +30200,55 @@
         <v>231.10000000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="5:5">
+    <row r="17" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="5:5">
+    <row r="18" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="5:5">
+    <row r="19" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E19" s="5"/>
     </row>
   </sheetData>
@@ -30265,15 +30265,15 @@
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>79</v>
       </c>
@@ -30299,7 +30299,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="2:9">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>25</v>
       </c>
@@ -30313,7 +30313,7 @@
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
     </row>
-    <row r="4" spans="2:9">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>9</v>
       </c>
@@ -30332,7 +30332,7 @@
       </c>
       <c r="I4" s="6"/>
     </row>
-    <row r="5" spans="2:9">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>88</v>
       </c>
@@ -30349,7 +30349,7 @@
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
     </row>
-    <row r="6" spans="2:9">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>89</v>
       </c>
@@ -30366,7 +30366,7 @@
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
     </row>
-    <row r="7" spans="2:9">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>84</v>
       </c>
@@ -30384,7 +30384,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="8" spans="2:9">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>92</v>
       </c>
@@ -30398,7 +30398,7 @@
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
     </row>
-    <row r="9" spans="2:9">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>17</v>
       </c>
@@ -30411,7 +30411,7 @@
         <v>267.90000000000003</v>
       </c>
     </row>
-    <row r="10" spans="2:9">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>93</v>
       </c>
@@ -30420,7 +30420,7 @@
         <v>2411.2899999999995</v>
       </c>
     </row>
-    <row r="12" spans="2:9">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>16</v>
       </c>
@@ -30428,7 +30428,7 @@
         <v>2679</v>
       </c>
     </row>
-    <row r="13" spans="2:9">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>17</v>
       </c>
@@ -30455,15 +30455,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DD052F9F6DEDAF408208614EE6C0588E" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="78b1a871d3837bbf4b54d4503b17fde3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c3fed6a1-161a-40e2-8029-a56ff5784305" xmlns:ns3="a44c0d7f-4a78-4b51-b7b2-4685f44aea4a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b16f68b41039dbc77ff33c189e465722" ns2:_="" ns3:_="">
     <xsd:import namespace="c3fed6a1-161a-40e2-8029-a56ff5784305"/>
@@ -30652,14 +30643,49 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E03034F-2412-4003-859C-DB1AF0725160}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E03034F-2412-4003-859C-DB1AF0725160}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a44c0d7f-4a78-4b51-b7b2-4685f44aea4a"/>
+    <ds:schemaRef ds:uri="c3fed6a1-161a-40e2-8029-a56ff5784305"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F5E3DEC-EE97-4492-972F-312F1B5FD0A6}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{217181BF-0E2C-4383-A509-B1B8BA24BF3A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="c3fed6a1-161a-40e2-8029-a56ff5784305"/>
+    <ds:schemaRef ds:uri="a44c0d7f-4a78-4b51-b7b2-4685f44aea4a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{217181BF-0E2C-4383-A509-B1B8BA24BF3A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F5E3DEC-EE97-4492-972F-312F1B5FD0A6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>